<commit_message>
Implement Windows for all major exploration areas, added more enemies/armor/weapons, general cleanup
</commit_message>
<xml_diff>
--- a/Sulimn.xlsx
+++ b/Sulimn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\C#\Projects\Sulimn-WPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\C#\Projects\WPF\Sulimn-WPF\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
   <si>
     <t>Damage</t>
   </si>
@@ -44,9 +44,6 @@
     <t>Skill Points</t>
   </si>
   <si>
-    <t>+  2(Level) - 1</t>
-  </si>
-  <si>
     <t>Armor</t>
   </si>
   <si>
@@ -66,6 +63,18 @@
   </si>
   <si>
     <t>+  5(Level &gt; 20)</t>
+  </si>
+  <si>
+    <t>Exp/Gold</t>
+  </si>
+  <si>
+    <t>+  2(Level - 1)</t>
+  </si>
+  <si>
+    <t>25(Level)</t>
+  </si>
+  <si>
+    <t>100(Level &gt;= 20)</t>
   </si>
 </sst>
 </file>
@@ -117,7 +126,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -129,6 +138,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -411,42 +423,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.625" customWidth="1"/>
-    <col min="4" max="5" width="12.625" customWidth="1"/>
-    <col min="7" max="8" width="12.625" customWidth="1"/>
+    <col min="1" max="2" width="13.625" customWidth="1"/>
+    <col min="4" max="5" width="13.625" customWidth="1"/>
+    <col min="6" max="6" width="9" customWidth="1"/>
+    <col min="7" max="8" width="13.625" customWidth="1"/>
+    <col min="10" max="11" width="13.625" customWidth="1"/>
+    <col min="13" max="14" width="13.625" customWidth="1"/>
+    <col min="16" max="17" width="13.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2"/>
-      <c r="M1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="N1" s="2"/>
-    </row>
-    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="5"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="5"/>
+      <c r="J1" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="5"/>
+      <c r="M1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N1" s="5"/>
+      <c r="P1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="5"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -459,26 +480,33 @@
       <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
+      <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="N2" s="3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="P2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -491,26 +519,33 @@
       <c r="E3" s="1">
         <v>30</v>
       </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="1">
         <v>1</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1">
+        <v>1</v>
+      </c>
+      <c r="K3" s="1">
         <v>30</v>
       </c>
-      <c r="J3" s="1">
-        <v>1</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="M3" s="1">
+        <v>1</v>
+      </c>
+      <c r="N3" s="1">
         <v>5</v>
       </c>
-      <c r="M3" s="1">
-        <v>1</v>
-      </c>
-      <c r="N3" s="1">
+      <c r="P3" s="1">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>30</v>
       </c>
@@ -521,28 +556,35 @@
         <v>2</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="F4" s="4"/>
       <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1">
+        <v>25</v>
+      </c>
+      <c r="J4" s="1">
         <v>30</v>
       </c>
-      <c r="H4" s="1">
+      <c r="K4" s="1">
         <v>50</v>
       </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>50</v>
       </c>
-      <c r="K4" s="1">
+      <c r="N4" s="1">
         <v>10</v>
       </c>
-      <c r="M4" s="1">
+      <c r="P4" s="1">
         <v>100</v>
       </c>
-      <c r="N4" s="4">
+      <c r="Q4" s="4">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>100</v>
       </c>
@@ -555,38 +597,102 @@
       <c r="E5" s="1">
         <v>38</v>
       </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="1">
+        <v>10</v>
+      </c>
+      <c r="H5" s="1">
+        <v>250</v>
+      </c>
+      <c r="J5" s="1">
         <v>100</v>
       </c>
-      <c r="H5" s="1">
+      <c r="K5" s="1">
         <v>100</v>
       </c>
-      <c r="J5" s="1"/>
-      <c r="K5" s="1"/>
-      <c r="M5" s="1">
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="P5" s="1">
         <v>500</v>
       </c>
-      <c r="N5" s="1">
+      <c r="Q5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
       <c r="D6" s="1">
+        <v>19</v>
+      </c>
+      <c r="E6" s="1">
+        <v>66</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1">
         <v>20</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="H6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D7" s="1">
+        <v>20</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="4"/>
+      <c r="G7" s="1">
+        <v>20</v>
+      </c>
+      <c r="H7" s="1">
+        <v>600</v>
+      </c>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D8" s="1">
+        <v>21</v>
+      </c>
+      <c r="E8" s="1">
+        <v>78</v>
+      </c>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1">
+        <v>21</v>
+      </c>
+      <c r="H8" s="1">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="D9" s="1">
+        <v>22</v>
+      </c>
+      <c r="E9" s="1">
+        <v>85</v>
+      </c>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
-    <mergeCell ref="G1:H1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="M1:N1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="G1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Alpha 2.2 - Some modifications
Finally added data binding on the Blackjack Window. Fixed a couple bugs
in some of the shop Windows, added several new Rings, a new set of
armor. Started working on a few methods to (hopefully) significantly
lower line count with several repetitive methods.
</commit_message>
<xml_diff>
--- a/Sulimn.xlsx
+++ b/Sulimn.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\C#\Projects\WPF\Sulimn-WPF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Programming\C#\Projects\WPF\Sulimn\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="23">
   <si>
     <t>Damage</t>
   </si>
@@ -75,6 +75,24 @@
   </si>
   <si>
     <t>100(Level &gt;= 20)</t>
+  </si>
+  <si>
+    <t>Rings</t>
+  </si>
+  <si>
+    <t>1 of 1 Type</t>
+  </si>
+  <si>
+    <t>2 of 1 Type</t>
+  </si>
+  <si>
+    <t>1 of 2 Types</t>
+  </si>
+  <si>
+    <t>1 of 3 Types</t>
+  </si>
+  <si>
+    <t>1 of 4 Types</t>
   </si>
 </sst>
 </file>
@@ -126,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -141,6 +159,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,21 +444,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q9"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="S2" sqref="S2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.625" customWidth="1"/>
-    <col min="4" max="5" width="13.625" customWidth="1"/>
+    <col min="1" max="2" width="13.5703125" customWidth="1"/>
+    <col min="4" max="5" width="13.5703125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="8" width="13.625" customWidth="1"/>
-    <col min="10" max="11" width="13.625" customWidth="1"/>
-    <col min="13" max="14" width="13.625" customWidth="1"/>
-    <col min="16" max="17" width="13.625" customWidth="1"/>
+    <col min="7" max="8" width="13.5703125" customWidth="1"/>
+    <col min="10" max="11" width="13.5703125" customWidth="1"/>
+    <col min="13" max="14" width="13.5703125" customWidth="1"/>
+    <col min="16" max="17" width="13.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
@@ -685,8 +706,63 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
+    <row r="11" spans="1:17" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="5"/>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="6">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6">
+        <v>16000</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="A11:B11"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="J1:K1"/>

</xml_diff>